<commit_message>
Created vinyl chloride distillation files, tested them with test_interface.py and started the main VCDistillation.py file
</commit_message>
<xml_diff>
--- a/FlashOperation/results.xlsx
+++ b/FlashOperation/results.xlsx
@@ -465,18 +465,18 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>40790632.85283854</v>
+        <v>45861701.46629615</v>
       </c>
       <c r="C2" t="n">
-        <v>2371.442624048322</v>
+        <v>3178.151334576864</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[ 3.30428962 11.60902993]</t>
+          <t>[5.85108711 1.04025955]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>46.14334559440613</v>
+        <v>28.20407700538635</v>
       </c>
     </row>
     <row r="3">
@@ -484,18 +484,18 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>3947.594394710895</v>
+        <v>3017.796647366936</v>
       </c>
       <c r="C3" t="n">
-        <v>1845.354112651814</v>
+        <v>2880.12358130603</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[ 4.16446647 11.01966926]</t>
+          <t>[ 2.71314885 18.76493152]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>46.14334559440613</v>
+        <v>28.20407700538635</v>
       </c>
     </row>
     <row r="4">
@@ -503,18 +503,18 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>2674.161252230549</v>
+        <v>2821.567765789802</v>
       </c>
       <c r="C4" t="n">
-        <v>1845.354112651814</v>
+        <v>2480.582326825271</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[ 4.16446647 11.01966926]</t>
+          <t>[ 3.16108031 18.79074714]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>46.14334559440613</v>
+        <v>28.20407700538635</v>
       </c>
     </row>
     <row r="5">
@@ -522,18 +522,18 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>2008.902244080716</v>
+        <v>2724.360496048061</v>
       </c>
       <c r="C5" t="n">
-        <v>1713.080687008202</v>
+        <v>2480.582326825271</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[4.86563974 4.03591674]</t>
+          <t>[ 3.16108031 18.79074714]</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>46.14334559440613</v>
+        <v>28.20407700538635</v>
       </c>
     </row>
     <row r="6">
@@ -541,18 +541,18 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>1855.495117623008</v>
+        <v>2448.458099808952</v>
       </c>
       <c r="C6" t="n">
-        <v>1608.081936633879</v>
+        <v>1920.205556846319</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[5.42754904 4.03591674]</t>
+          <t>[ 4.0256312  18.76574977]</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>46.14334559440613</v>
+        <v>28.20407700538635</v>
       </c>
     </row>
     <row r="7">
@@ -560,18 +560,18 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>1787.852732884652</v>
+        <v>2207.000191106167</v>
       </c>
       <c r="C7" t="n">
-        <v>1608.081936633879</v>
+        <v>1865.070504249676</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[5.42754904 4.03591674]</t>
+          <t>[ 4.13078268 18.78928727]</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>46.14334559440613</v>
+        <v>28.20407700538635</v>
       </c>
     </row>
     <row r="8">
@@ -579,18 +579,18 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>1641.641186133636</v>
+        <v>1883.101198075768</v>
       </c>
       <c r="C8" t="n">
-        <v>1309.692223494936</v>
+        <v>1820.389134475256</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>[8.53293594 3.98146802]</t>
+          <t>[ 4.22105208 18.91704751]</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>46.14334559440613</v>
+        <v>28.20407700538635</v>
       </c>
     </row>
     <row r="9">
@@ -598,18 +598,18 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>1526.934355109307</v>
+        <v>1870.437056700439</v>
       </c>
       <c r="C9" t="n">
-        <v>1249.876702417805</v>
+        <v>1820.389134475256</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>[10.20254912  3.98146802]</t>
+          <t>[ 4.22105208 18.91704751]</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>46.14334559440613</v>
+        <v>28.20407700538635</v>
       </c>
     </row>
     <row r="10">
@@ -617,18 +617,18 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>1435.712365142419</v>
+        <v>1870.437056700439</v>
       </c>
       <c r="C10" t="n">
-        <v>1249.136655996367</v>
+        <v>1820.389134475256</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[10.23122802  3.9816277 ]</t>
+          <t>[ 4.22105208 18.91704751]</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>46.14334559440613</v>
+        <v>28.20407700538635</v>
       </c>
     </row>
     <row r="11">
@@ -636,18 +636,18 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>1330.200024109853</v>
+        <v>1852.012089934923</v>
       </c>
       <c r="C11" t="n">
-        <v>1247.308998718997</v>
+        <v>1819.561961136669</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>[10.32619731  3.98146802]</t>
+          <t>[ 4.22105208 18.93284487]</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>46.14334559440613</v>
+        <v>28.20407700538635</v>
       </c>
     </row>
   </sheetData>

</xml_diff>